<commit_message>
Correcting a bug in hydrocomputation
</commit_message>
<xml_diff>
--- a/Examples/Output Example.xlsx
+++ b/Examples/Output Example.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Pt</t>
   </si>
@@ -275,6 +275,12 @@
   </si>
   <si>
     <t>ρsw</t>
+  </si>
+  <si>
+    <t>https://github.com/akira215/HydroCpp</t>
+  </si>
+  <si>
+    <t>Repo:</t>
   </si>
 </sst>
 </file>
@@ -26205,6 +26211,28 @@
         <v>74</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>